<commit_message>
Ajout majuscule nom des sous-familles
</commit_message>
<xml_diff>
--- a/docs/base_de_donnees_materiaux/bdd_materiaux_v4.1.xlsx
+++ b/docs/base_de_donnees_materiaux/bdd_materiaux_v4.1.xlsx
@@ -128,7 +128,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Prix minimal que le materiau peut prendre,
 il est calculé automatiquement.
@@ -143,7 +143,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Prix dans une base 1, on divise le prix par 1 euro pour ne plus avoir d'unité.
 </t>
@@ -168,7 +168,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -376,7 +376,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Prix minimal que le materiau peut prendre,
 il est calculé automatiquement.
@@ -391,7 +391,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Prix dans une base 1, on divise le prix par 1 euro pour ne plus avoir d'unité.
 </t>
@@ -416,7 +416,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -1447,28 +1447,28 @@
     <t>Résistance à la corrosion</t>
   </si>
   <si>
-    <t>steel for generale engineering purposes</t>
-  </si>
-  <si>
-    <t>free cutting steels</t>
-  </si>
-  <si>
-    <t>case hardening steels</t>
-  </si>
-  <si>
-    <t>steels for quenching and tempering</t>
-  </si>
-  <si>
-    <t>martensitic stainless steels</t>
-  </si>
-  <si>
-    <t>austenitic stainless steels</t>
-  </si>
-  <si>
-    <t>ferritic stainless steels</t>
-  </si>
-  <si>
     <t xml:space="preserve">Base de données Matériaux de l'IPOC AT-OMC v4.1 </t>
+  </si>
+  <si>
+    <t>Free cutting steels</t>
+  </si>
+  <si>
+    <t>Steel for general engineering purposes</t>
+  </si>
+  <si>
+    <t>Case hardening steels</t>
+  </si>
+  <si>
+    <t>Steels for quenching and tempering</t>
+  </si>
+  <si>
+    <t>Austenitic stainless steels</t>
+  </si>
+  <si>
+    <t>Martensitic stainless steels</t>
+  </si>
+  <si>
+    <t>Ferritic stainless steels</t>
   </si>
 </sst>
 </file>
@@ -1478,7 +1478,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1621,19 +1621,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
     <font>
       <i/>
@@ -2500,72 +2487,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="9" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2609,6 +2563,39 @@
     <xf numFmtId="14" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Heading 2b" xfId="6"/>
@@ -2623,9 +2610,6 @@
     <cellStyle name="Titre 4 2" xfId="7"/>
   </cellStyles>
   <dxfs count="82">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -3092,6 +3076,9 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
       <fill>
         <patternFill patternType="solid">
@@ -3445,30 +3432,30 @@
       <calculatedColumnFormula>IF(N6&lt;&gt;0,(O6-N6)/(N6+O6),IF(K6&lt;&gt;0,((1+M6)^(YEAR(TODAY())-YEAR(L6))-1)/((1+M6)^(YEAR(TODAY())-YEAR(L6))+1),"-"))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" name="Usinabilité"/>
-    <tableColumn id="6" name="% outillage" dataDxfId="0"/>
+    <tableColumn id="6" name="% outillage" dataDxfId="57"/>
     <tableColumn id="7" name="Dureté en Hb"/>
     <tableColumn id="8" name="Rm en Mpa"/>
     <tableColumn id="9" name="Rp0.2 en Mpa"/>
     <tableColumn id="10" name="A%"/>
-    <tableColumn id="11" name="Aptitude à la soudure" dataDxfId="57">
+    <tableColumn id="11" name="Aptitude à la soudure" dataDxfId="56">
       <calculatedColumnFormula>IF(AM6&lt;0.4,1,IF(AM6&lt;0.7,2,3))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Traitement thermique" dataDxfId="56"/>
-    <tableColumn id="13" name="Aptitude au traitement thermique" dataDxfId="55"/>
-    <tableColumn id="28" name="Résistance à la corrosion" dataDxfId="54"/>
-    <tableColumn id="14" name="C" dataDxfId="53"/>
-    <tableColumn id="15" name="Si" dataDxfId="52"/>
-    <tableColumn id="16" name="Mn" dataDxfId="51"/>
-    <tableColumn id="17" name="P" dataDxfId="50"/>
-    <tableColumn id="18" name="S" dataDxfId="49"/>
-    <tableColumn id="19" name="N" dataDxfId="48"/>
-    <tableColumn id="20" name="Cr" dataDxfId="47"/>
-    <tableColumn id="21" name="Mo" dataDxfId="46"/>
-    <tableColumn id="22" name="Ni" dataDxfId="45"/>
-    <tableColumn id="23" name="Pb" dataDxfId="44"/>
-    <tableColumn id="24" name="B" dataDxfId="43"/>
-    <tableColumn id="25" name="V" dataDxfId="42"/>
-    <tableColumn id="26" name="Ceq" dataDxfId="41">
+    <tableColumn id="12" name="Traitement thermique" dataDxfId="55"/>
+    <tableColumn id="13" name="Aptitude au traitement thermique" dataDxfId="54"/>
+    <tableColumn id="28" name="Résistance à la corrosion" dataDxfId="53"/>
+    <tableColumn id="14" name="C" dataDxfId="52"/>
+    <tableColumn id="15" name="Si" dataDxfId="51"/>
+    <tableColumn id="16" name="Mn" dataDxfId="50"/>
+    <tableColumn id="17" name="P" dataDxfId="49"/>
+    <tableColumn id="18" name="S" dataDxfId="48"/>
+    <tableColumn id="19" name="N" dataDxfId="47"/>
+    <tableColumn id="20" name="Cr" dataDxfId="46"/>
+    <tableColumn id="21" name="Mo" dataDxfId="45"/>
+    <tableColumn id="22" name="Ni" dataDxfId="44"/>
+    <tableColumn id="23" name="Pb" dataDxfId="43"/>
+    <tableColumn id="24" name="B" dataDxfId="42"/>
+    <tableColumn id="25" name="V" dataDxfId="41"/>
+    <tableColumn id="26" name="Ceq" dataDxfId="40">
       <calculatedColumnFormula>AA6+AC6/6+(AG6+AH6+AL6)/5+AI6/15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3477,58 +3464,58 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="B5:AL34" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39" tableBorderDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="B5:AL34" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38" tableBorderDxfId="37">
   <autoFilter ref="B5:AL34"/>
   <tableColumns count="37">
-    <tableColumn id="1" name="Famille" dataDxfId="37"/>
-    <tableColumn id="2" name="nuance" dataDxfId="36"/>
-    <tableColumn id="4" name="Numéro" dataDxfId="35"/>
-    <tableColumn id="5" name="Indice prix tonne" dataDxfId="34"/>
-    <tableColumn id="38" name="prix min" dataDxfId="33">
+    <tableColumn id="1" name="Famille" dataDxfId="36"/>
+    <tableColumn id="2" name="nuance" dataDxfId="35"/>
+    <tableColumn id="4" name="Numéro" dataDxfId="34"/>
+    <tableColumn id="5" name="Indice prix tonne" dataDxfId="33"/>
+    <tableColumn id="38" name="prix min" dataDxfId="32">
       <calculatedColumnFormula>IF(J6&lt;&gt;"-",J6*(1-P6),"-")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="37" name="indice prix" dataDxfId="32">
+    <tableColumn id="37" name="indice prix" dataDxfId="31">
       <calculatedColumnFormula>J6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="36" name="prix max" dataDxfId="31">
+    <tableColumn id="36" name="prix max" dataDxfId="30">
       <calculatedColumnFormula>IF(J6&lt;&gt;"-",J6*(1+P6),"-")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="35" name="prix réel 2018" dataDxfId="30">
+    <tableColumn id="35" name="prix réel 2018" dataDxfId="29">
       <calculatedColumnFormula>IF(YEAR(L6)=YEAR(TODAY()),K6,IF(AND(N6=0,K6=0),"-","n/a"))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="33" name="prix estimé 2018" dataDxfId="29">
+    <tableColumn id="33" name="prix estimé 2018" dataDxfId="28">
       <calculatedColumnFormula>IF(K6&lt;&gt;0,(K6*(1+M6)^(YEAR(TODAY())-YEAR(L6))+K6)/2,IF(N6&lt;&gt;0,(N6+O6)/2,"-"))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="32" name="dernier prix connu" dataDxfId="28"/>
-    <tableColumn id="31" name="date d'application du dernier prix" dataDxfId="27"/>
-    <tableColumn id="30" name="taux d'inflation" dataDxfId="26" dataCellStyle="Pourcentage"/>
-    <tableColumn id="29" name="prix min internet" dataDxfId="25"/>
-    <tableColumn id="28" name="prix max internet" dataDxfId="24"/>
-    <tableColumn id="3" name="incertitude prix" dataDxfId="23" dataCellStyle="Pourcentage">
+    <tableColumn id="32" name="dernier prix connu" dataDxfId="27"/>
+    <tableColumn id="31" name="date d'application du dernier prix" dataDxfId="26"/>
+    <tableColumn id="30" name="taux d'inflation" dataDxfId="25" dataCellStyle="Pourcentage"/>
+    <tableColumn id="29" name="prix min internet" dataDxfId="24"/>
+    <tableColumn id="28" name="prix max internet" dataDxfId="23"/>
+    <tableColumn id="3" name="incertitude prix" dataDxfId="22" dataCellStyle="Pourcentage">
       <calculatedColumnFormula>IF(N6&lt;&gt;0,(O6-N6)/(N6+O6),IF(K6&lt;&gt;0,((1+M6)^(YEAR(TODAY())-YEAR(L6))-1)/((1+M6)^(YEAR(TODAY())-YEAR(L6))+1),"-"))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Usinabilité" dataDxfId="22"/>
-    <tableColumn id="7" name="% outillage" dataDxfId="21" dataCellStyle="Pourcentage"/>
-    <tableColumn id="8" name="Dureté en Hb" dataDxfId="20"/>
-    <tableColumn id="9" name="Rm en Mpa" dataDxfId="19"/>
-    <tableColumn id="10" name="Rp0.2 en Mpa" dataDxfId="18"/>
-    <tableColumn id="11" name="A% " dataDxfId="17"/>
-    <tableColumn id="12" name="Aptitude à la soudure" dataDxfId="16"/>
-    <tableColumn id="13" name="Traitement thermique" dataDxfId="15"/>
-    <tableColumn id="14" name="Aptitude au traitement thermique" dataDxfId="14"/>
-    <tableColumn id="15" name="résistance à la corrosion" dataDxfId="13"/>
-    <tableColumn id="16" name="C" dataDxfId="12"/>
-    <tableColumn id="17" name="Si" dataDxfId="11"/>
-    <tableColumn id="18" name="Mn" dataDxfId="10"/>
-    <tableColumn id="19" name="P" dataDxfId="9"/>
-    <tableColumn id="20" name="S" dataDxfId="8"/>
-    <tableColumn id="21" name="N" dataDxfId="7"/>
-    <tableColumn id="22" name="Cr" dataDxfId="6"/>
-    <tableColumn id="23" name="Mo" dataDxfId="5"/>
-    <tableColumn id="24" name="Ni" dataDxfId="4"/>
-    <tableColumn id="25" name="Pb" dataDxfId="3"/>
-    <tableColumn id="26" name="B" dataDxfId="2"/>
-    <tableColumn id="27" name="V" dataDxfId="1"/>
+    <tableColumn id="6" name="Usinabilité" dataDxfId="21"/>
+    <tableColumn id="7" name="% outillage" dataDxfId="20" dataCellStyle="Pourcentage"/>
+    <tableColumn id="8" name="Dureté en Hb" dataDxfId="19"/>
+    <tableColumn id="9" name="Rm en Mpa" dataDxfId="18"/>
+    <tableColumn id="10" name="Rp0.2 en Mpa" dataDxfId="17"/>
+    <tableColumn id="11" name="A% " dataDxfId="16"/>
+    <tableColumn id="12" name="Aptitude à la soudure" dataDxfId="15"/>
+    <tableColumn id="13" name="Traitement thermique" dataDxfId="14"/>
+    <tableColumn id="14" name="Aptitude au traitement thermique" dataDxfId="13"/>
+    <tableColumn id="15" name="résistance à la corrosion" dataDxfId="12"/>
+    <tableColumn id="16" name="C" dataDxfId="11"/>
+    <tableColumn id="17" name="Si" dataDxfId="10"/>
+    <tableColumn id="18" name="Mn" dataDxfId="9"/>
+    <tableColumn id="19" name="P" dataDxfId="8"/>
+    <tableColumn id="20" name="S" dataDxfId="7"/>
+    <tableColumn id="21" name="N" dataDxfId="6"/>
+    <tableColumn id="22" name="Cr" dataDxfId="5"/>
+    <tableColumn id="23" name="Mo" dataDxfId="4"/>
+    <tableColumn id="24" name="Ni" dataDxfId="3"/>
+    <tableColumn id="25" name="Pb" dataDxfId="2"/>
+    <tableColumn id="26" name="B" dataDxfId="1"/>
+    <tableColumn id="27" name="V" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3844,245 +3831,245 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="286" t="s">
-        <v>256</v>
-      </c>
-      <c r="B1" s="286"/>
-      <c r="C1" s="286"/>
-      <c r="D1" s="286"/>
-      <c r="E1" s="286"/>
-      <c r="F1" s="286"/>
-      <c r="G1" s="286"/>
-      <c r="H1" s="286"/>
-      <c r="I1" s="286"/>
+      <c r="A1" s="318" t="s">
+        <v>249</v>
+      </c>
+      <c r="B1" s="318"/>
+      <c r="C1" s="318"/>
+      <c r="D1" s="318"/>
+      <c r="E1" s="318"/>
+      <c r="F1" s="318"/>
+      <c r="G1" s="318"/>
+      <c r="H1" s="318"/>
+      <c r="I1" s="318"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="286"/>
-      <c r="B2" s="286"/>
-      <c r="C2" s="286"/>
-      <c r="D2" s="286"/>
-      <c r="E2" s="286"/>
-      <c r="F2" s="286"/>
-      <c r="G2" s="286"/>
-      <c r="H2" s="286"/>
-      <c r="I2" s="286"/>
+      <c r="A2" s="318"/>
+      <c r="B2" s="318"/>
+      <c r="C2" s="318"/>
+      <c r="D2" s="318"/>
+      <c r="E2" s="318"/>
+      <c r="F2" s="318"/>
+      <c r="G2" s="318"/>
+      <c r="H2" s="318"/>
+      <c r="I2" s="318"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="286"/>
-      <c r="B3" s="286"/>
-      <c r="C3" s="286"/>
-      <c r="D3" s="286"/>
-      <c r="E3" s="286"/>
-      <c r="F3" s="286"/>
-      <c r="G3" s="286"/>
-      <c r="H3" s="286"/>
-      <c r="I3" s="286"/>
+      <c r="A3" s="318"/>
+      <c r="B3" s="318"/>
+      <c r="C3" s="318"/>
+      <c r="D3" s="318"/>
+      <c r="E3" s="318"/>
+      <c r="F3" s="318"/>
+      <c r="G3" s="318"/>
+      <c r="H3" s="318"/>
+      <c r="I3" s="318"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="286"/>
-      <c r="B4" s="286"/>
-      <c r="C4" s="286"/>
-      <c r="D4" s="286"/>
-      <c r="E4" s="286"/>
-      <c r="F4" s="286"/>
-      <c r="G4" s="286"/>
-      <c r="H4" s="286"/>
-      <c r="I4" s="286"/>
+      <c r="A4" s="318"/>
+      <c r="B4" s="318"/>
+      <c r="C4" s="318"/>
+      <c r="D4" s="318"/>
+      <c r="E4" s="318"/>
+      <c r="F4" s="318"/>
+      <c r="G4" s="318"/>
+      <c r="H4" s="318"/>
+      <c r="I4" s="318"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="286"/>
-      <c r="B5" s="286"/>
-      <c r="C5" s="286"/>
-      <c r="D5" s="286"/>
-      <c r="E5" s="286"/>
-      <c r="F5" s="286"/>
-      <c r="G5" s="286"/>
-      <c r="H5" s="286"/>
-      <c r="I5" s="286"/>
+      <c r="A5" s="318"/>
+      <c r="B5" s="318"/>
+      <c r="C5" s="318"/>
+      <c r="D5" s="318"/>
+      <c r="E5" s="318"/>
+      <c r="F5" s="318"/>
+      <c r="G5" s="318"/>
+      <c r="H5" s="318"/>
+      <c r="I5" s="318"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="286"/>
-      <c r="B6" s="286"/>
-      <c r="C6" s="286"/>
-      <c r="D6" s="286"/>
-      <c r="E6" s="286"/>
-      <c r="F6" s="286"/>
-      <c r="G6" s="286"/>
-      <c r="H6" s="286"/>
-      <c r="I6" s="286"/>
+      <c r="A6" s="318"/>
+      <c r="B6" s="318"/>
+      <c r="C6" s="318"/>
+      <c r="D6" s="318"/>
+      <c r="E6" s="318"/>
+      <c r="F6" s="318"/>
+      <c r="G6" s="318"/>
+      <c r="H6" s="318"/>
+      <c r="I6" s="318"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="286"/>
-      <c r="B7" s="286"/>
-      <c r="C7" s="286"/>
-      <c r="D7" s="286"/>
-      <c r="E7" s="286"/>
-      <c r="F7" s="286"/>
-      <c r="G7" s="286"/>
-      <c r="H7" s="286"/>
-      <c r="I7" s="286"/>
+      <c r="A7" s="318"/>
+      <c r="B7" s="318"/>
+      <c r="C7" s="318"/>
+      <c r="D7" s="318"/>
+      <c r="E7" s="318"/>
+      <c r="F7" s="318"/>
+      <c r="G7" s="318"/>
+      <c r="H7" s="318"/>
+      <c r="I7" s="318"/>
     </row>
     <row r="8" spans="1:9" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="286"/>
-      <c r="B8" s="286"/>
-      <c r="C8" s="286"/>
-      <c r="D8" s="286"/>
-      <c r="E8" s="286"/>
-      <c r="F8" s="286"/>
-      <c r="G8" s="286"/>
-      <c r="H8" s="286"/>
-      <c r="I8" s="286"/>
+      <c r="A8" s="318"/>
+      <c r="B8" s="318"/>
+      <c r="C8" s="318"/>
+      <c r="D8" s="318"/>
+      <c r="E8" s="318"/>
+      <c r="F8" s="318"/>
+      <c r="G8" s="318"/>
+      <c r="H8" s="318"/>
+      <c r="I8" s="318"/>
     </row>
     <row r="9" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="287" t="s">
+      <c r="A9" s="319" t="s">
         <v>231</v>
       </c>
-      <c r="B9" s="287"/>
-      <c r="C9" s="287"/>
-      <c r="D9" s="287"/>
-      <c r="E9" s="287"/>
-      <c r="F9" s="287"/>
-      <c r="G9" s="287"/>
-      <c r="H9" s="287"/>
-      <c r="I9" s="287"/>
+      <c r="B9" s="319"/>
+      <c r="C9" s="319"/>
+      <c r="D9" s="319"/>
+      <c r="E9" s="319"/>
+      <c r="F9" s="319"/>
+      <c r="G9" s="319"/>
+      <c r="H9" s="319"/>
+      <c r="I9" s="319"/>
     </row>
     <row r="10" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="287"/>
-      <c r="B10" s="287"/>
-      <c r="C10" s="287"/>
-      <c r="D10" s="287"/>
-      <c r="E10" s="287"/>
-      <c r="F10" s="287"/>
-      <c r="G10" s="287"/>
-      <c r="H10" s="287"/>
-      <c r="I10" s="287"/>
+      <c r="A10" s="319"/>
+      <c r="B10" s="319"/>
+      <c r="C10" s="319"/>
+      <c r="D10" s="319"/>
+      <c r="E10" s="319"/>
+      <c r="F10" s="319"/>
+      <c r="G10" s="319"/>
+      <c r="H10" s="319"/>
+      <c r="I10" s="319"/>
     </row>
     <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="288" t="s">
+      <c r="A11" s="320" t="s">
         <v>170</v>
       </c>
-      <c r="B11" s="288"/>
-      <c r="C11" s="288"/>
-      <c r="D11" s="288"/>
-      <c r="E11" s="288"/>
-      <c r="F11" s="288"/>
-      <c r="G11" s="288"/>
-      <c r="H11" s="288"/>
-      <c r="I11" s="288"/>
+      <c r="B11" s="320"/>
+      <c r="C11" s="320"/>
+      <c r="D11" s="320"/>
+      <c r="E11" s="320"/>
+      <c r="F11" s="320"/>
+      <c r="G11" s="320"/>
+      <c r="H11" s="320"/>
+      <c r="I11" s="320"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="288"/>
-      <c r="B12" s="288"/>
-      <c r="C12" s="288"/>
-      <c r="D12" s="288"/>
-      <c r="E12" s="288"/>
-      <c r="F12" s="288"/>
-      <c r="G12" s="288"/>
-      <c r="H12" s="288"/>
-      <c r="I12" s="288"/>
+      <c r="A12" s="320"/>
+      <c r="B12" s="320"/>
+      <c r="C12" s="320"/>
+      <c r="D12" s="320"/>
+      <c r="E12" s="320"/>
+      <c r="F12" s="320"/>
+      <c r="G12" s="320"/>
+      <c r="H12" s="320"/>
+      <c r="I12" s="320"/>
     </row>
     <row r="13" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="288"/>
-      <c r="B13" s="288"/>
-      <c r="C13" s="288"/>
-      <c r="D13" s="288"/>
-      <c r="E13" s="288"/>
-      <c r="F13" s="288"/>
-      <c r="G13" s="288"/>
-      <c r="H13" s="288"/>
-      <c r="I13" s="288"/>
+      <c r="A13" s="320"/>
+      <c r="B13" s="320"/>
+      <c r="C13" s="320"/>
+      <c r="D13" s="320"/>
+      <c r="E13" s="320"/>
+      <c r="F13" s="320"/>
+      <c r="G13" s="320"/>
+      <c r="H13" s="320"/>
+      <c r="I13" s="320"/>
     </row>
     <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="288" t="s">
+      <c r="A14" s="320" t="s">
         <v>232</v>
       </c>
-      <c r="B14" s="288"/>
-      <c r="C14" s="288"/>
-      <c r="D14" s="288"/>
-      <c r="E14" s="288"/>
-      <c r="F14" s="288"/>
-      <c r="G14" s="288"/>
-      <c r="H14" s="288"/>
-      <c r="I14" s="288"/>
+      <c r="B14" s="320"/>
+      <c r="C14" s="320"/>
+      <c r="D14" s="320"/>
+      <c r="E14" s="320"/>
+      <c r="F14" s="320"/>
+      <c r="G14" s="320"/>
+      <c r="H14" s="320"/>
+      <c r="I14" s="320"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="288"/>
-      <c r="B15" s="288"/>
-      <c r="C15" s="288"/>
-      <c r="D15" s="288"/>
-      <c r="E15" s="288"/>
-      <c r="F15" s="288"/>
-      <c r="G15" s="288"/>
-      <c r="H15" s="288"/>
-      <c r="I15" s="288"/>
+      <c r="A15" s="320"/>
+      <c r="B15" s="320"/>
+      <c r="C15" s="320"/>
+      <c r="D15" s="320"/>
+      <c r="E15" s="320"/>
+      <c r="F15" s="320"/>
+      <c r="G15" s="320"/>
+      <c r="H15" s="320"/>
+      <c r="I15" s="320"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="288"/>
-      <c r="B16" s="288"/>
-      <c r="C16" s="288"/>
-      <c r="D16" s="288"/>
-      <c r="E16" s="288"/>
-      <c r="F16" s="288"/>
-      <c r="G16" s="288"/>
-      <c r="H16" s="288"/>
-      <c r="I16" s="288"/>
+      <c r="A16" s="320"/>
+      <c r="B16" s="320"/>
+      <c r="C16" s="320"/>
+      <c r="D16" s="320"/>
+      <c r="E16" s="320"/>
+      <c r="F16" s="320"/>
+      <c r="G16" s="320"/>
+      <c r="H16" s="320"/>
+      <c r="I16" s="320"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="289" t="s">
+      <c r="A17" s="321" t="s">
         <v>244</v>
       </c>
-      <c r="B17" s="289"/>
-      <c r="C17" s="289"/>
-      <c r="D17" s="289"/>
-      <c r="E17" s="289"/>
-      <c r="F17" s="289"/>
-      <c r="G17" s="289"/>
-      <c r="H17" s="289"/>
-      <c r="I17" s="289"/>
+      <c r="B17" s="321"/>
+      <c r="C17" s="321"/>
+      <c r="D17" s="321"/>
+      <c r="E17" s="321"/>
+      <c r="F17" s="321"/>
+      <c r="G17" s="321"/>
+      <c r="H17" s="321"/>
+      <c r="I17" s="321"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="289"/>
-      <c r="B18" s="289"/>
-      <c r="C18" s="289"/>
-      <c r="D18" s="289"/>
-      <c r="E18" s="289"/>
-      <c r="F18" s="289"/>
-      <c r="G18" s="289"/>
-      <c r="H18" s="289"/>
-      <c r="I18" s="289"/>
+      <c r="A18" s="321"/>
+      <c r="B18" s="321"/>
+      <c r="C18" s="321"/>
+      <c r="D18" s="321"/>
+      <c r="E18" s="321"/>
+      <c r="F18" s="321"/>
+      <c r="G18" s="321"/>
+      <c r="H18" s="321"/>
+      <c r="I18" s="321"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="289"/>
-      <c r="B19" s="289"/>
-      <c r="C19" s="289"/>
-      <c r="D19" s="289"/>
-      <c r="E19" s="289"/>
-      <c r="F19" s="289"/>
-      <c r="G19" s="289"/>
-      <c r="H19" s="289"/>
-      <c r="I19" s="289"/>
+      <c r="A19" s="321"/>
+      <c r="B19" s="321"/>
+      <c r="C19" s="321"/>
+      <c r="D19" s="321"/>
+      <c r="E19" s="321"/>
+      <c r="F19" s="321"/>
+      <c r="G19" s="321"/>
+      <c r="H19" s="321"/>
+      <c r="I19" s="321"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="289"/>
-      <c r="B20" s="289"/>
-      <c r="C20" s="289"/>
-      <c r="D20" s="289"/>
-      <c r="E20" s="289"/>
-      <c r="F20" s="289"/>
-      <c r="G20" s="289"/>
-      <c r="H20" s="289"/>
-      <c r="I20" s="289"/>
+      <c r="A20" s="321"/>
+      <c r="B20" s="321"/>
+      <c r="C20" s="321"/>
+      <c r="D20" s="321"/>
+      <c r="E20" s="321"/>
+      <c r="F20" s="321"/>
+      <c r="G20" s="321"/>
+      <c r="H20" s="321"/>
+      <c r="I20" s="321"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="289"/>
-      <c r="B21" s="289"/>
-      <c r="C21" s="289"/>
-      <c r="D21" s="289"/>
-      <c r="E21" s="289"/>
-      <c r="F21" s="289"/>
-      <c r="G21" s="289"/>
-      <c r="H21" s="289"/>
-      <c r="I21" s="289"/>
+      <c r="A21" s="321"/>
+      <c r="B21" s="321"/>
+      <c r="C21" s="321"/>
+      <c r="D21" s="321"/>
+      <c r="E21" s="321"/>
+      <c r="F21" s="321"/>
+      <c r="G21" s="321"/>
+      <c r="H21" s="321"/>
+      <c r="I21" s="321"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -4104,11 +4091,11 @@
   <dimension ref="B1:AN79"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="N59" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="N62" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="A6" sqref="A6"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="R79" sqref="R79"/>
+      <selection pane="bottomRight" activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4146,36 +4133,36 @@
         <v>165</v>
       </c>
       <c r="R3"/>
-      <c r="AA3" s="290" t="s">
+      <c r="AA3" s="322" t="s">
         <v>155</v>
       </c>
-      <c r="AB3" s="290"/>
-      <c r="AC3" s="290"/>
-      <c r="AD3" s="290"/>
-      <c r="AE3" s="290"/>
-      <c r="AF3" s="290"/>
-      <c r="AG3" s="290"/>
-      <c r="AH3" s="290"/>
-      <c r="AI3" s="290"/>
-      <c r="AJ3" s="290"/>
-      <c r="AK3" s="290"/>
-      <c r="AL3" s="290"/>
-      <c r="AM3" s="290"/>
+      <c r="AB3" s="322"/>
+      <c r="AC3" s="322"/>
+      <c r="AD3" s="322"/>
+      <c r="AE3" s="322"/>
+      <c r="AF3" s="322"/>
+      <c r="AG3" s="322"/>
+      <c r="AH3" s="322"/>
+      <c r="AI3" s="322"/>
+      <c r="AJ3" s="322"/>
+      <c r="AK3" s="322"/>
+      <c r="AL3" s="322"/>
+      <c r="AM3" s="322"/>
     </row>
     <row r="4" spans="2:40" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AA4" s="291"/>
-      <c r="AB4" s="291"/>
-      <c r="AC4" s="291"/>
-      <c r="AD4" s="291"/>
-      <c r="AE4" s="291"/>
-      <c r="AF4" s="291"/>
-      <c r="AG4" s="291"/>
-      <c r="AH4" s="291"/>
-      <c r="AI4" s="291"/>
-      <c r="AJ4" s="291"/>
-      <c r="AK4" s="291"/>
-      <c r="AL4" s="291"/>
-      <c r="AM4" s="291"/>
+      <c r="AA4" s="323"/>
+      <c r="AB4" s="323"/>
+      <c r="AC4" s="323"/>
+      <c r="AD4" s="323"/>
+      <c r="AE4" s="323"/>
+      <c r="AF4" s="323"/>
+      <c r="AG4" s="323"/>
+      <c r="AH4" s="323"/>
+      <c r="AI4" s="323"/>
+      <c r="AJ4" s="323"/>
+      <c r="AK4" s="323"/>
+      <c r="AL4" s="323"/>
+      <c r="AM4" s="323"/>
     </row>
     <row r="5" spans="2:40" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="265" t="s">
@@ -4296,7 +4283,7 @@
     </row>
     <row r="6" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C6" s="16" t="s">
         <v>5</v>
@@ -4341,7 +4328,7 @@
       <c r="Q6" s="18">
         <v>50</v>
       </c>
-      <c r="R6" s="304">
+      <c r="R6" s="293">
         <v>5</v>
       </c>
       <c r="S6" s="19">
@@ -4456,7 +4443,7 @@
       <c r="Q7" s="11">
         <v>50</v>
       </c>
-      <c r="R7" s="303">
+      <c r="R7" s="292">
         <v>5</v>
       </c>
       <c r="S7" s="10">
@@ -4571,7 +4558,7 @@
       <c r="Q8" s="20">
         <v>50</v>
       </c>
-      <c r="R8" s="304">
+      <c r="R8" s="293">
         <v>5</v>
       </c>
       <c r="S8" s="19">
@@ -4686,7 +4673,7 @@
       <c r="Q9" s="11">
         <v>50</v>
       </c>
-      <c r="R9" s="303">
+      <c r="R9" s="292">
         <v>5</v>
       </c>
       <c r="S9" s="10">
@@ -4801,7 +4788,7 @@
       <c r="Q10" s="18">
         <v>50</v>
       </c>
-      <c r="R10" s="304">
+      <c r="R10" s="293">
         <v>5</v>
       </c>
       <c r="S10" s="19">
@@ -4916,7 +4903,7 @@
       <c r="Q11" s="11">
         <v>57</v>
       </c>
-      <c r="R11" s="303">
+      <c r="R11" s="292">
         <v>5</v>
       </c>
       <c r="S11" s="10">
@@ -5033,7 +5020,7 @@
       <c r="Q12" s="19">
         <v>57</v>
       </c>
-      <c r="R12" s="304">
+      <c r="R12" s="293">
         <v>5</v>
       </c>
       <c r="S12" s="19">
@@ -5144,7 +5131,7 @@
       <c r="Q13" s="9">
         <v>50</v>
       </c>
-      <c r="R13" s="303">
+      <c r="R13" s="292">
         <v>5</v>
       </c>
       <c r="S13" s="10">
@@ -5259,7 +5246,7 @@
       <c r="Q14" s="18">
         <v>47</v>
       </c>
-      <c r="R14" s="304">
+      <c r="R14" s="293">
         <v>5</v>
       </c>
       <c r="S14" s="19">
@@ -5374,7 +5361,7 @@
       <c r="Q15" s="11">
         <v>45</v>
       </c>
-      <c r="R15" s="303">
+      <c r="R15" s="292">
         <v>5</v>
       </c>
       <c r="S15" s="10">
@@ -5485,7 +5472,7 @@
       <c r="Q16" s="20">
         <v>42</v>
       </c>
-      <c r="R16" s="304">
+      <c r="R16" s="293">
         <v>5</v>
       </c>
       <c r="S16" s="19">
@@ -5596,7 +5583,7 @@
       <c r="Q17" s="14">
         <v>41</v>
       </c>
-      <c r="R17" s="314">
+      <c r="R17" s="303">
         <v>5</v>
       </c>
       <c r="S17" s="15">
@@ -5713,7 +5700,7 @@
       <c r="Q18" s="23">
         <v>100</v>
       </c>
-      <c r="R18" s="305">
+      <c r="R18" s="294">
         <v>5</v>
       </c>
       <c r="S18" s="24">
@@ -5828,7 +5815,7 @@
       <c r="Q19" s="37">
         <v>115</v>
       </c>
-      <c r="R19" s="315">
+      <c r="R19" s="304">
         <v>5</v>
       </c>
       <c r="S19" s="38">
@@ -5943,7 +5930,7 @@
       <c r="Q20" s="28">
         <v>110</v>
       </c>
-      <c r="R20" s="307">
+      <c r="R20" s="296">
         <v>5</v>
       </c>
       <c r="S20" s="25">
@@ -6058,7 +6045,7 @@
       <c r="Q21" s="37">
         <v>130</v>
       </c>
-      <c r="R21" s="315">
+      <c r="R21" s="304">
         <v>5</v>
       </c>
       <c r="S21" s="38">
@@ -6173,7 +6160,7 @@
       <c r="Q22" s="28">
         <v>95</v>
       </c>
-      <c r="R22" s="307">
+      <c r="R22" s="296">
         <v>5</v>
       </c>
       <c r="S22" s="25">
@@ -6288,7 +6275,7 @@
       <c r="Q23" s="37">
         <v>105</v>
       </c>
-      <c r="R23" s="315">
+      <c r="R23" s="304">
         <v>5</v>
       </c>
       <c r="S23" s="38">
@@ -6403,7 +6390,7 @@
       <c r="Q24" s="29">
         <v>95</v>
       </c>
-      <c r="R24" s="307">
+      <c r="R24" s="296">
         <v>5</v>
       </c>
       <c r="S24" s="25">
@@ -6518,7 +6505,7 @@
       <c r="Q25" s="37">
         <v>75</v>
       </c>
-      <c r="R25" s="315">
+      <c r="R25" s="304">
         <v>5</v>
       </c>
       <c r="S25" s="38">
@@ -6633,7 +6620,7 @@
       <c r="Q26" s="28">
         <v>95</v>
       </c>
-      <c r="R26" s="307">
+      <c r="R26" s="296">
         <v>5</v>
       </c>
       <c r="S26" s="25">
@@ -6748,7 +6735,7 @@
       <c r="Q27" s="39">
         <v>75</v>
       </c>
-      <c r="R27" s="315">
+      <c r="R27" s="304">
         <v>5</v>
       </c>
       <c r="S27" s="38">
@@ -6863,7 +6850,7 @@
       <c r="Q28" s="29">
         <v>90</v>
       </c>
-      <c r="R28" s="307">
+      <c r="R28" s="296">
         <v>5</v>
       </c>
       <c r="S28" s="25">
@@ -6978,7 +6965,7 @@
       <c r="Q29" s="37">
         <v>65</v>
       </c>
-      <c r="R29" s="315">
+      <c r="R29" s="304">
         <v>5</v>
       </c>
       <c r="S29" s="38">
@@ -7093,7 +7080,7 @@
       <c r="Q30" s="28">
         <v>80</v>
       </c>
-      <c r="R30" s="307">
+      <c r="R30" s="296">
         <v>5</v>
       </c>
       <c r="S30" s="25">
@@ -7208,7 +7195,7 @@
       <c r="Q31" s="37">
         <v>62</v>
       </c>
-      <c r="R31" s="315">
+      <c r="R31" s="304">
         <v>5</v>
       </c>
       <c r="S31" s="38">
@@ -7321,7 +7308,7 @@
       <c r="Q32" s="29">
         <v>80</v>
       </c>
-      <c r="R32" s="307">
+      <c r="R32" s="296">
         <v>5</v>
       </c>
       <c r="S32" s="25">
@@ -7434,7 +7421,7 @@
       <c r="Q33" s="39">
         <v>75</v>
       </c>
-      <c r="R33" s="315">
+      <c r="R33" s="304">
         <v>5</v>
       </c>
       <c r="S33" s="38">
@@ -7547,7 +7534,7 @@
       <c r="Q34" s="29">
         <v>75</v>
       </c>
-      <c r="R34" s="307">
+      <c r="R34" s="296">
         <v>5</v>
       </c>
       <c r="S34" s="25">
@@ -7660,7 +7647,7 @@
       <c r="Q35" s="39">
         <v>80</v>
       </c>
-      <c r="R35" s="315">
+      <c r="R35" s="304">
         <v>5</v>
       </c>
       <c r="S35" s="38">
@@ -7775,7 +7762,7 @@
       <c r="Q36" s="28">
         <v>75</v>
       </c>
-      <c r="R36" s="307">
+      <c r="R36" s="296">
         <v>5</v>
       </c>
       <c r="S36" s="25">
@@ -7890,7 +7877,7 @@
       <c r="Q37" s="37">
         <v>67</v>
       </c>
-      <c r="R37" s="315">
+      <c r="R37" s="304">
         <v>5</v>
       </c>
       <c r="S37" s="38">
@@ -8005,7 +7992,7 @@
       <c r="Q38" s="33">
         <v>85</v>
       </c>
-      <c r="R38" s="316">
+      <c r="R38" s="305">
         <v>5</v>
       </c>
       <c r="S38" s="34">
@@ -8077,7 +8064,7 @@
     </row>
     <row r="39" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B39" s="3" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C39" s="42" t="s">
         <v>64</v>
@@ -8122,7 +8109,7 @@
       <c r="Q39" s="44">
         <v>65</v>
       </c>
-      <c r="R39" s="311">
+      <c r="R39" s="300">
         <v>5</v>
       </c>
       <c r="S39" s="45">
@@ -8237,7 +8224,7 @@
       <c r="Q40" s="57">
         <v>67</v>
       </c>
-      <c r="R40" s="312">
+      <c r="R40" s="301">
         <v>5</v>
       </c>
       <c r="S40" s="58">
@@ -8352,7 +8339,7 @@
       <c r="Q41" s="49">
         <v>67</v>
       </c>
-      <c r="R41" s="317">
+      <c r="R41" s="306">
         <v>5</v>
       </c>
       <c r="S41" s="46">
@@ -8467,7 +8454,7 @@
       <c r="Q42" s="57">
         <v>60</v>
       </c>
-      <c r="R42" s="312">
+      <c r="R42" s="301">
         <v>7</v>
       </c>
       <c r="S42" s="58">
@@ -8582,7 +8569,7 @@
       <c r="Q43" s="50">
         <v>70</v>
       </c>
-      <c r="R43" s="317">
+      <c r="R43" s="306">
         <v>7</v>
       </c>
       <c r="S43" s="46">
@@ -8699,7 +8686,7 @@
       <c r="Q44" s="59">
         <v>65</v>
       </c>
-      <c r="R44" s="312">
+      <c r="R44" s="301">
         <v>7</v>
       </c>
       <c r="S44" s="58">
@@ -8814,7 +8801,7 @@
       <c r="Q45" s="50">
         <v>70</v>
       </c>
-      <c r="R45" s="317">
+      <c r="R45" s="306">
         <v>7</v>
       </c>
       <c r="S45" s="46">
@@ -8929,7 +8916,7 @@
       <c r="Q46" s="57">
         <v>70</v>
       </c>
-      <c r="R46" s="312">
+      <c r="R46" s="301">
         <v>7</v>
       </c>
       <c r="S46" s="58">
@@ -9044,7 +9031,7 @@
       <c r="Q47" s="50">
         <v>60</v>
       </c>
-      <c r="R47" s="317">
+      <c r="R47" s="306">
         <v>7</v>
       </c>
       <c r="S47" s="46">
@@ -9159,7 +9146,7 @@
       <c r="Q48" s="57">
         <v>62</v>
       </c>
-      <c r="R48" s="312">
+      <c r="R48" s="301">
         <v>7</v>
       </c>
       <c r="S48" s="58">
@@ -9274,7 +9261,7 @@
       <c r="Q49" s="53">
         <v>60</v>
       </c>
-      <c r="R49" s="318">
+      <c r="R49" s="307">
         <v>7</v>
       </c>
       <c r="S49" s="54">
@@ -9346,7 +9333,7 @@
     </row>
     <row r="50" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B50" s="4" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C50" s="60" t="s">
         <v>84</v>
@@ -9391,7 +9378,7 @@
       <c r="Q50" s="63">
         <v>55</v>
       </c>
-      <c r="R50" s="319">
+      <c r="R50" s="308">
         <v>7</v>
       </c>
       <c r="S50" s="64">
@@ -9506,7 +9493,7 @@
       <c r="Q51" s="74">
         <v>67</v>
       </c>
-      <c r="R51" s="320">
+      <c r="R51" s="309">
         <v>5</v>
       </c>
       <c r="S51" s="73">
@@ -9621,7 +9608,7 @@
       <c r="Q52" s="66">
         <v>53</v>
       </c>
-      <c r="R52" s="321">
+      <c r="R52" s="310">
         <v>7</v>
       </c>
       <c r="S52" s="65">
@@ -9736,7 +9723,7 @@
       <c r="Q53" s="74">
         <v>65</v>
       </c>
-      <c r="R53" s="320">
+      <c r="R53" s="309">
         <v>5</v>
       </c>
       <c r="S53" s="73">
@@ -9851,7 +9838,7 @@
       <c r="Q54" s="67">
         <v>53</v>
       </c>
-      <c r="R54" s="321">
+      <c r="R54" s="310">
         <v>7</v>
       </c>
       <c r="S54" s="65">
@@ -9966,7 +9953,7 @@
       <c r="Q55" s="74">
         <v>65</v>
       </c>
-      <c r="R55" s="320">
+      <c r="R55" s="309">
         <v>5</v>
       </c>
       <c r="S55" s="73">
@@ -10081,7 +10068,7 @@
       <c r="Q56" s="66">
         <v>48</v>
       </c>
-      <c r="R56" s="321">
+      <c r="R56" s="310">
         <v>7</v>
       </c>
       <c r="S56" s="65">
@@ -10196,7 +10183,7 @@
       <c r="Q57" s="74">
         <v>60</v>
       </c>
-      <c r="R57" s="320">
+      <c r="R57" s="309">
         <v>5</v>
       </c>
       <c r="S57" s="73">
@@ -10311,7 +10298,7 @@
       <c r="Q58" s="67">
         <v>45</v>
       </c>
-      <c r="R58" s="321">
+      <c r="R58" s="310">
         <v>7</v>
       </c>
       <c r="S58" s="65">
@@ -10426,7 +10413,7 @@
       <c r="Q59" s="74">
         <v>57</v>
       </c>
-      <c r="R59" s="320">
+      <c r="R59" s="309">
         <v>5</v>
       </c>
       <c r="S59" s="73">
@@ -10541,7 +10528,7 @@
       <c r="Q60" s="67">
         <v>45</v>
       </c>
-      <c r="R60" s="321">
+      <c r="R60" s="310">
         <v>5</v>
       </c>
       <c r="S60" s="65">
@@ -10656,7 +10643,7 @@
       <c r="Q61" s="74">
         <v>55</v>
       </c>
-      <c r="R61" s="320">
+      <c r="R61" s="309">
         <v>7</v>
       </c>
       <c r="S61" s="73">
@@ -10771,7 +10758,7 @@
       <c r="Q62" s="69">
         <v>40</v>
       </c>
-      <c r="R62" s="322">
+      <c r="R62" s="311">
         <v>10</v>
       </c>
       <c r="S62" s="65">
@@ -10886,7 +10873,7 @@
       <c r="Q63" s="75">
         <v>45</v>
       </c>
-      <c r="R63" s="320">
+      <c r="R63" s="309">
         <v>7</v>
       </c>
       <c r="S63" s="73">
@@ -10999,7 +10986,7 @@
       <c r="Q64" s="66">
         <v>38</v>
       </c>
-      <c r="R64" s="321">
+      <c r="R64" s="310">
         <v>10</v>
       </c>
       <c r="S64" s="65">
@@ -11114,7 +11101,7 @@
       <c r="Q65" s="74">
         <v>68</v>
       </c>
-      <c r="R65" s="320">
+      <c r="R65" s="309">
         <v>7</v>
       </c>
       <c r="S65" s="73">
@@ -11229,7 +11216,7 @@
       <c r="Q66" s="66">
         <v>55</v>
       </c>
-      <c r="R66" s="321">
+      <c r="R66" s="310">
         <v>10</v>
       </c>
       <c r="S66" s="65">
@@ -11344,7 +11331,7 @@
       <c r="Q67" s="75">
         <v>58</v>
       </c>
-      <c r="R67" s="320">
+      <c r="R67" s="309">
         <v>7</v>
       </c>
       <c r="S67" s="73">
@@ -11459,7 +11446,7 @@
       <c r="Q68" s="66">
         <v>50</v>
       </c>
-      <c r="R68" s="321">
+      <c r="R68" s="310">
         <v>10</v>
       </c>
       <c r="S68" s="65">
@@ -11574,7 +11561,7 @@
       <c r="Q69" s="74">
         <v>37</v>
       </c>
-      <c r="R69" s="320">
+      <c r="R69" s="309">
         <v>7</v>
       </c>
       <c r="S69" s="73">
@@ -11689,7 +11676,7 @@
       <c r="Q70" s="66">
         <v>46</v>
       </c>
-      <c r="R70" s="321">
+      <c r="R70" s="310">
         <v>7</v>
       </c>
       <c r="S70" s="65">
@@ -11804,7 +11791,7 @@
       <c r="Q71" s="81">
         <v>40</v>
       </c>
-      <c r="R71" s="323">
+      <c r="R71" s="312">
         <v>10</v>
       </c>
       <c r="S71" s="73">
@@ -11919,7 +11906,7 @@
       <c r="Q72" s="66">
         <v>40</v>
       </c>
-      <c r="R72" s="321">
+      <c r="R72" s="310">
         <v>7</v>
       </c>
       <c r="S72" s="65">
@@ -12034,7 +12021,7 @@
       <c r="Q73" s="81">
         <v>40</v>
       </c>
-      <c r="R73" s="323">
+      <c r="R73" s="312">
         <v>10</v>
       </c>
       <c r="S73" s="73">
@@ -12149,7 +12136,7 @@
       <c r="Q74" s="67">
         <v>48</v>
       </c>
-      <c r="R74" s="321">
+      <c r="R74" s="310">
         <v>7</v>
       </c>
       <c r="S74" s="65">
@@ -12264,7 +12251,7 @@
       <c r="Q75" s="74">
         <v>46</v>
       </c>
-      <c r="R75" s="320">
+      <c r="R75" s="309">
         <v>10</v>
       </c>
       <c r="S75" s="73">
@@ -12379,7 +12366,7 @@
       <c r="Q76" s="66">
         <v>37</v>
       </c>
-      <c r="R76" s="321">
+      <c r="R76" s="310">
         <v>10</v>
       </c>
       <c r="S76" s="65">
@@ -12492,7 +12479,7 @@
       <c r="Q77" s="75">
         <v>45</v>
       </c>
-      <c r="R77" s="324">
+      <c r="R77" s="313">
         <v>10</v>
       </c>
       <c r="S77" s="87">
@@ -12607,7 +12594,7 @@
       <c r="Q78" s="66">
         <v>35</v>
       </c>
-      <c r="R78" s="325">
+      <c r="R78" s="314">
         <v>12</v>
       </c>
       <c r="S78" s="83">
@@ -12698,11 +12685,11 @@
   <dimension ref="B1:AN71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="E18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="K31" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="A6" sqref="A6"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="N36" sqref="N36"/>
+      <selection pane="bottomRight" activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -12715,7 +12702,7 @@
     <col min="14" max="15" width="11" style="216"/>
     <col min="16" max="16" width="11" style="239"/>
     <col min="17" max="17" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11" style="297"/>
+    <col min="18" max="18" width="11" style="286"/>
     <col min="19" max="19" width="11" style="79"/>
     <col min="22" max="23" width="12" customWidth="1"/>
     <col min="24" max="24" width="14.375" style="106" customWidth="1"/>
@@ -12745,35 +12732,35 @@
       </c>
       <c r="D3" s="1"/>
       <c r="S3"/>
-      <c r="AA3" s="292" t="s">
+      <c r="AA3" s="324" t="s">
         <v>155</v>
       </c>
-      <c r="AB3" s="293"/>
-      <c r="AC3" s="293"/>
-      <c r="AD3" s="293"/>
-      <c r="AE3" s="293"/>
-      <c r="AF3" s="293"/>
-      <c r="AG3" s="293"/>
-      <c r="AH3" s="293"/>
-      <c r="AI3" s="293"/>
-      <c r="AJ3" s="293"/>
-      <c r="AK3" s="293"/>
-      <c r="AL3" s="294"/>
+      <c r="AB3" s="325"/>
+      <c r="AC3" s="325"/>
+      <c r="AD3" s="325"/>
+      <c r="AE3" s="325"/>
+      <c r="AF3" s="325"/>
+      <c r="AG3" s="325"/>
+      <c r="AH3" s="325"/>
+      <c r="AI3" s="325"/>
+      <c r="AJ3" s="325"/>
+      <c r="AK3" s="325"/>
+      <c r="AL3" s="326"/>
       <c r="AM3" s="187"/>
     </row>
     <row r="4" spans="2:39" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AA4" s="295"/>
-      <c r="AB4" s="291"/>
-      <c r="AC4" s="291"/>
-      <c r="AD4" s="291"/>
-      <c r="AE4" s="291"/>
-      <c r="AF4" s="291"/>
-      <c r="AG4" s="291"/>
-      <c r="AH4" s="291"/>
-      <c r="AI4" s="291"/>
-      <c r="AJ4" s="291"/>
-      <c r="AK4" s="291"/>
-      <c r="AL4" s="296"/>
+      <c r="AA4" s="327"/>
+      <c r="AB4" s="323"/>
+      <c r="AC4" s="323"/>
+      <c r="AD4" s="323"/>
+      <c r="AE4" s="323"/>
+      <c r="AF4" s="323"/>
+      <c r="AG4" s="323"/>
+      <c r="AH4" s="323"/>
+      <c r="AI4" s="323"/>
+      <c r="AJ4" s="323"/>
+      <c r="AK4" s="323"/>
+      <c r="AL4" s="328"/>
       <c r="AM4" s="187"/>
     </row>
     <row r="5" spans="2:39" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12825,7 +12812,7 @@
       <c r="Q5" s="127" t="s">
         <v>3</v>
       </c>
-      <c r="R5" s="298" t="s">
+      <c r="R5" s="287" t="s">
         <v>148</v>
       </c>
       <c r="S5" s="259" t="s">
@@ -12937,7 +12924,7 @@
       <c r="Q6" s="102">
         <v>30</v>
       </c>
-      <c r="R6" s="303">
+      <c r="R6" s="292">
         <v>10</v>
       </c>
       <c r="S6" s="10">
@@ -13048,7 +13035,7 @@
       <c r="Q7" s="124">
         <v>25</v>
       </c>
-      <c r="R7" s="304">
+      <c r="R7" s="293">
         <v>10</v>
       </c>
       <c r="S7" s="19">
@@ -13159,7 +13146,7 @@
       <c r="Q8" s="118">
         <v>65</v>
       </c>
-      <c r="R8" s="303">
+      <c r="R8" s="292">
         <v>10</v>
       </c>
       <c r="S8" s="10">
@@ -13269,7 +13256,7 @@
       <c r="Q9" s="93">
         <v>40</v>
       </c>
-      <c r="R9" s="304">
+      <c r="R9" s="293">
         <v>10</v>
       </c>
       <c r="S9" s="19">
@@ -13380,7 +13367,7 @@
       <c r="Q10" s="118">
         <v>45</v>
       </c>
-      <c r="R10" s="303">
+      <c r="R10" s="292">
         <v>10</v>
       </c>
       <c r="S10" s="10">
@@ -13491,7 +13478,7 @@
       <c r="Q11" s="116">
         <v>45</v>
       </c>
-      <c r="R11" s="304">
+      <c r="R11" s="293">
         <v>10</v>
       </c>
       <c r="S11" s="19">
@@ -13602,7 +13589,7 @@
       <c r="Q12" s="102">
         <v>40</v>
       </c>
-      <c r="R12" s="303">
+      <c r="R12" s="292">
         <v>10</v>
       </c>
       <c r="S12" s="10">
@@ -13713,7 +13700,7 @@
       <c r="Q13" s="92">
         <v>40</v>
       </c>
-      <c r="R13" s="304">
+      <c r="R13" s="293">
         <v>10</v>
       </c>
       <c r="S13" s="19">
@@ -13824,7 +13811,7 @@
       <c r="Q14" s="105">
         <v>40</v>
       </c>
-      <c r="R14" s="303">
+      <c r="R14" s="292">
         <v>10</v>
       </c>
       <c r="S14" s="10">
@@ -13935,7 +13922,7 @@
       <c r="Q15" s="100">
         <v>35</v>
       </c>
-      <c r="R15" s="304">
+      <c r="R15" s="293">
         <v>10</v>
       </c>
       <c r="S15" s="19">
@@ -14045,7 +14032,7 @@
       <c r="Q16" s="99">
         <v>35</v>
       </c>
-      <c r="R16" s="303">
+      <c r="R16" s="292">
         <v>10</v>
       </c>
       <c r="S16" s="10">
@@ -14156,7 +14143,7 @@
       <c r="Q17" s="93">
         <v>45</v>
       </c>
-      <c r="R17" s="304">
+      <c r="R17" s="293">
         <v>10</v>
       </c>
       <c r="S17" s="19">
@@ -14267,7 +14254,7 @@
       <c r="Q18" s="134">
         <v>65</v>
       </c>
-      <c r="R18" s="303">
+      <c r="R18" s="292">
         <v>10</v>
       </c>
       <c r="S18" s="10">
@@ -14378,7 +14365,7 @@
       <c r="Q19" s="92">
         <v>20</v>
       </c>
-      <c r="R19" s="304">
+      <c r="R19" s="293">
         <v>10</v>
       </c>
       <c r="S19" s="19">
@@ -14445,7 +14432,7 @@
     </row>
     <row r="20" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B20" s="159" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="C20" s="21" t="s">
         <v>188</v>
@@ -14490,7 +14477,7 @@
       <c r="Q20" s="101">
         <v>90</v>
       </c>
-      <c r="R20" s="305">
+      <c r="R20" s="294">
         <v>10</v>
       </c>
       <c r="S20" s="24">
@@ -14587,7 +14574,7 @@
       <c r="K21" s="246">
         <v>2905</v>
       </c>
-      <c r="L21" s="326">
+      <c r="L21" s="315">
         <v>43282</v>
       </c>
       <c r="M21" s="247"/>
@@ -14600,7 +14587,7 @@
       <c r="Q21" s="146">
         <v>45</v>
       </c>
-      <c r="R21" s="306">
+      <c r="R21" s="295">
         <v>10</v>
       </c>
       <c r="S21" s="141">
@@ -14697,7 +14684,7 @@
       <c r="K22" s="248">
         <v>2905</v>
       </c>
-      <c r="L22" s="328">
+      <c r="L22" s="317">
         <v>43282</v>
       </c>
       <c r="M22" s="226"/>
@@ -14710,7 +14697,7 @@
       <c r="Q22" s="94">
         <v>35</v>
       </c>
-      <c r="R22" s="307">
+      <c r="R22" s="296">
         <v>10</v>
       </c>
       <c r="S22" s="25">
@@ -14807,7 +14794,7 @@
       <c r="K23" s="246">
         <v>2652</v>
       </c>
-      <c r="L23" s="326">
+      <c r="L23" s="315">
         <v>43282</v>
       </c>
       <c r="M23" s="247"/>
@@ -14820,7 +14807,7 @@
       <c r="Q23" s="140">
         <v>50</v>
       </c>
-      <c r="R23" s="306">
+      <c r="R23" s="295">
         <v>10</v>
       </c>
       <c r="S23" s="141">
@@ -14930,7 +14917,7 @@
       <c r="Q24" s="94">
         <v>45</v>
       </c>
-      <c r="R24" s="307">
+      <c r="R24" s="296">
         <v>10</v>
       </c>
       <c r="S24" s="25">
@@ -15040,7 +15027,7 @@
       <c r="Q25" s="147">
         <v>55</v>
       </c>
-      <c r="R25" s="306">
+      <c r="R25" s="295">
         <v>10</v>
       </c>
       <c r="S25" s="141">
@@ -15150,7 +15137,7 @@
       <c r="Q26" s="136">
         <v>35</v>
       </c>
-      <c r="R26" s="308">
+      <c r="R26" s="297">
         <v>12</v>
       </c>
       <c r="S26" s="121">
@@ -15260,7 +15247,7 @@
       <c r="Q27" s="150">
         <v>42</v>
       </c>
-      <c r="R27" s="309">
+      <c r="R27" s="298">
         <v>10</v>
       </c>
       <c r="S27" s="151">
@@ -15370,7 +15357,7 @@
       <c r="Q28" s="136">
         <v>47</v>
       </c>
-      <c r="R28" s="308">
+      <c r="R28" s="297">
         <v>10</v>
       </c>
       <c r="S28" s="121">
@@ -15480,7 +15467,7 @@
       <c r="Q29" s="146">
         <v>45</v>
       </c>
-      <c r="R29" s="306">
+      <c r="R29" s="295">
         <v>10</v>
       </c>
       <c r="S29" s="141">
@@ -15591,7 +15578,7 @@
       <c r="Q30" s="117">
         <v>30</v>
       </c>
-      <c r="R30" s="307">
+      <c r="R30" s="296">
         <v>12</v>
       </c>
       <c r="S30" s="25">
@@ -15701,7 +15688,7 @@
       <c r="Q31" s="146">
         <v>55</v>
       </c>
-      <c r="R31" s="310">
+      <c r="R31" s="299">
         <v>10</v>
       </c>
       <c r="S31" s="141">
@@ -15769,7 +15756,7 @@
     </row>
     <row r="32" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B32" s="176" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C32" s="42" t="s">
         <v>197</v>
@@ -15814,7 +15801,7 @@
       <c r="Q32" s="177">
         <v>55</v>
       </c>
-      <c r="R32" s="311">
+      <c r="R32" s="300">
         <v>10</v>
       </c>
       <c r="S32" s="45">
@@ -15911,7 +15898,7 @@
       <c r="K33" s="253">
         <v>2421</v>
       </c>
-      <c r="L33" s="327">
+      <c r="L33" s="316">
         <v>43282</v>
       </c>
       <c r="M33" s="231"/>
@@ -15924,7 +15911,7 @@
       <c r="Q33" s="153">
         <v>75</v>
       </c>
-      <c r="R33" s="312">
+      <c r="R33" s="301">
         <v>10</v>
       </c>
       <c r="S33" s="58">
@@ -16035,7 +16022,7 @@
       <c r="Q34" s="183">
         <v>75</v>
       </c>
-      <c r="R34" s="313">
+      <c r="R34" s="302">
         <v>10</v>
       </c>
       <c r="S34" s="184">
@@ -16119,7 +16106,7 @@
       <c r="O35" s="256"/>
       <c r="P35" s="257"/>
       <c r="Q35" s="6"/>
-      <c r="R35" s="299"/>
+      <c r="R35" s="288"/>
       <c r="S35" s="131"/>
       <c r="T35" s="6"/>
       <c r="U35" s="6"/>
@@ -16160,7 +16147,7 @@
       <c r="O36" s="256"/>
       <c r="P36" s="257"/>
       <c r="Q36" s="6"/>
-      <c r="R36" s="300"/>
+      <c r="R36" s="289"/>
       <c r="S36" s="131"/>
       <c r="T36" s="6"/>
       <c r="U36" s="6"/>
@@ -16201,7 +16188,7 @@
       <c r="O37" s="256"/>
       <c r="P37" s="257"/>
       <c r="Q37" s="6"/>
-      <c r="R37" s="301"/>
+      <c r="R37" s="290"/>
       <c r="S37" s="131"/>
       <c r="T37" s="6"/>
       <c r="U37" s="6"/>
@@ -16242,7 +16229,7 @@
       <c r="O38" s="256"/>
       <c r="P38" s="257"/>
       <c r="Q38" s="6"/>
-      <c r="R38" s="301"/>
+      <c r="R38" s="290"/>
       <c r="S38" s="131"/>
       <c r="T38" s="6"/>
       <c r="U38" s="6"/>
@@ -16283,7 +16270,7 @@
       <c r="O39" s="256"/>
       <c r="P39" s="257"/>
       <c r="Q39" s="6"/>
-      <c r="R39" s="300"/>
+      <c r="R39" s="289"/>
       <c r="S39" s="131"/>
       <c r="T39" s="6"/>
       <c r="U39" s="6"/>
@@ -16324,7 +16311,7 @@
       <c r="O40" s="256"/>
       <c r="P40" s="257"/>
       <c r="Q40" s="6"/>
-      <c r="R40" s="301"/>
+      <c r="R40" s="290"/>
       <c r="S40" s="131"/>
       <c r="T40" s="6"/>
       <c r="U40" s="6"/>
@@ -16365,7 +16352,7 @@
       <c r="O41" s="256"/>
       <c r="P41" s="257"/>
       <c r="Q41" s="6"/>
-      <c r="R41" s="301"/>
+      <c r="R41" s="290"/>
       <c r="S41" s="131"/>
       <c r="T41" s="6"/>
       <c r="U41" s="6"/>
@@ -16406,7 +16393,7 @@
       <c r="O42" s="256"/>
       <c r="P42" s="257"/>
       <c r="Q42" s="6"/>
-      <c r="R42" s="301"/>
+      <c r="R42" s="290"/>
       <c r="S42" s="131"/>
       <c r="T42" s="6"/>
       <c r="U42" s="6"/>
@@ -16447,7 +16434,7 @@
       <c r="O43" s="256"/>
       <c r="P43" s="257"/>
       <c r="Q43" s="6"/>
-      <c r="R43" s="300"/>
+      <c r="R43" s="289"/>
       <c r="S43" s="131"/>
       <c r="T43" s="6"/>
       <c r="U43" s="6"/>
@@ -16488,7 +16475,7 @@
       <c r="O44" s="256"/>
       <c r="P44" s="257"/>
       <c r="Q44" s="6"/>
-      <c r="R44" s="301"/>
+      <c r="R44" s="290"/>
       <c r="S44" s="131"/>
       <c r="T44" s="6"/>
       <c r="U44" s="6"/>
@@ -16529,7 +16516,7 @@
       <c r="O45" s="256"/>
       <c r="P45" s="257"/>
       <c r="Q45" s="6"/>
-      <c r="R45" s="301"/>
+      <c r="R45" s="290"/>
       <c r="S45" s="131"/>
       <c r="T45" s="6"/>
       <c r="U45" s="6"/>
@@ -16570,7 +16557,7 @@
       <c r="O46" s="256"/>
       <c r="P46" s="257"/>
       <c r="Q46" s="6"/>
-      <c r="R46" s="301"/>
+      <c r="R46" s="290"/>
       <c r="S46" s="131"/>
       <c r="T46" s="6"/>
       <c r="U46" s="6"/>
@@ -16611,7 +16598,7 @@
       <c r="O47" s="256"/>
       <c r="P47" s="257"/>
       <c r="Q47" s="6"/>
-      <c r="R47" s="300"/>
+      <c r="R47" s="289"/>
       <c r="S47" s="131"/>
       <c r="T47" s="6"/>
       <c r="U47" s="6"/>
@@ -16652,7 +16639,7 @@
       <c r="O48" s="256"/>
       <c r="P48" s="257"/>
       <c r="Q48" s="6"/>
-      <c r="R48" s="301"/>
+      <c r="R48" s="290"/>
       <c r="S48" s="131"/>
       <c r="T48" s="6"/>
       <c r="U48" s="6"/>
@@ -16693,7 +16680,7 @@
       <c r="O49" s="256"/>
       <c r="P49" s="257"/>
       <c r="Q49" s="133"/>
-      <c r="R49" s="300"/>
+      <c r="R49" s="289"/>
       <c r="S49" s="131"/>
       <c r="T49" s="6"/>
       <c r="U49" s="6"/>
@@ -16734,7 +16721,7 @@
       <c r="O50" s="256"/>
       <c r="P50" s="257"/>
       <c r="Q50" s="6"/>
-      <c r="R50" s="301"/>
+      <c r="R50" s="290"/>
       <c r="S50" s="131"/>
       <c r="T50" s="6"/>
       <c r="U50" s="6"/>
@@ -16775,7 +16762,7 @@
       <c r="O51" s="256"/>
       <c r="P51" s="257"/>
       <c r="Q51" s="6"/>
-      <c r="R51" s="301"/>
+      <c r="R51" s="290"/>
       <c r="S51" s="131"/>
       <c r="T51" s="6"/>
       <c r="U51" s="6"/>
@@ -16816,7 +16803,7 @@
       <c r="O52" s="256"/>
       <c r="P52" s="257"/>
       <c r="Q52" s="6"/>
-      <c r="R52" s="300"/>
+      <c r="R52" s="289"/>
       <c r="S52" s="131"/>
       <c r="T52" s="6"/>
       <c r="U52" s="6"/>
@@ -16857,7 +16844,7 @@
       <c r="O53" s="256"/>
       <c r="P53" s="257"/>
       <c r="Q53" s="133"/>
-      <c r="R53" s="301"/>
+      <c r="R53" s="290"/>
       <c r="S53" s="131"/>
       <c r="T53" s="6"/>
       <c r="U53" s="6"/>
@@ -16898,7 +16885,7 @@
       <c r="O54" s="256"/>
       <c r="P54" s="257"/>
       <c r="Q54" s="6"/>
-      <c r="R54" s="301"/>
+      <c r="R54" s="290"/>
       <c r="S54" s="131"/>
       <c r="T54" s="6"/>
       <c r="U54" s="6"/>
@@ -16939,7 +16926,7 @@
       <c r="O55" s="256"/>
       <c r="P55" s="257"/>
       <c r="Q55" s="6"/>
-      <c r="R55" s="301"/>
+      <c r="R55" s="290"/>
       <c r="S55" s="131"/>
       <c r="T55" s="6"/>
       <c r="U55" s="6"/>
@@ -16980,7 +16967,7 @@
       <c r="O56" s="256"/>
       <c r="P56" s="257"/>
       <c r="Q56" s="6"/>
-      <c r="R56" s="300"/>
+      <c r="R56" s="289"/>
       <c r="S56" s="131"/>
       <c r="T56" s="6"/>
       <c r="U56" s="6"/>
@@ -17021,7 +17008,7 @@
       <c r="O57" s="256"/>
       <c r="P57" s="257"/>
       <c r="Q57" s="6"/>
-      <c r="R57" s="301"/>
+      <c r="R57" s="290"/>
       <c r="S57" s="131"/>
       <c r="T57" s="6"/>
       <c r="U57" s="6"/>
@@ -17062,7 +17049,7 @@
       <c r="O58" s="256"/>
       <c r="P58" s="257"/>
       <c r="Q58" s="133"/>
-      <c r="R58" s="301"/>
+      <c r="R58" s="290"/>
       <c r="S58" s="131"/>
       <c r="T58" s="6"/>
       <c r="U58" s="6"/>
@@ -17103,7 +17090,7 @@
       <c r="O59" s="256"/>
       <c r="P59" s="257"/>
       <c r="Q59" s="6"/>
-      <c r="R59" s="301"/>
+      <c r="R59" s="290"/>
       <c r="S59" s="131"/>
       <c r="T59" s="6"/>
       <c r="U59" s="6"/>
@@ -17144,7 +17131,7 @@
       <c r="O60" s="256"/>
       <c r="P60" s="257"/>
       <c r="Q60" s="6"/>
-      <c r="R60" s="301"/>
+      <c r="R60" s="290"/>
       <c r="S60" s="131"/>
       <c r="T60" s="6"/>
       <c r="U60" s="6"/>
@@ -17185,7 +17172,7 @@
       <c r="O61" s="258"/>
       <c r="P61" s="257"/>
       <c r="Q61" s="133"/>
-      <c r="R61" s="301"/>
+      <c r="R61" s="290"/>
       <c r="S61" s="131"/>
       <c r="T61" s="6"/>
       <c r="U61" s="6"/>
@@ -17226,7 +17213,7 @@
       <c r="O62" s="256"/>
       <c r="P62" s="257"/>
       <c r="Q62" s="6"/>
-      <c r="R62" s="301"/>
+      <c r="R62" s="290"/>
       <c r="S62" s="131"/>
       <c r="T62" s="6"/>
       <c r="U62" s="6"/>
@@ -17267,7 +17254,7 @@
       <c r="O63" s="256"/>
       <c r="P63" s="257"/>
       <c r="Q63" s="6"/>
-      <c r="R63" s="300"/>
+      <c r="R63" s="289"/>
       <c r="S63" s="131"/>
       <c r="T63" s="6"/>
       <c r="U63" s="6"/>
@@ -17308,7 +17295,7 @@
       <c r="O64" s="256"/>
       <c r="P64" s="257"/>
       <c r="Q64" s="6"/>
-      <c r="R64" s="301"/>
+      <c r="R64" s="290"/>
       <c r="S64" s="131"/>
       <c r="T64" s="6"/>
       <c r="U64" s="6"/>
@@ -17349,7 +17336,7 @@
       <c r="O65" s="256"/>
       <c r="P65" s="257"/>
       <c r="Q65" s="6"/>
-      <c r="R65" s="301"/>
+      <c r="R65" s="290"/>
       <c r="S65" s="131"/>
       <c r="T65" s="6"/>
       <c r="U65" s="6"/>
@@ -17390,7 +17377,7 @@
       <c r="O66" s="256"/>
       <c r="P66" s="257"/>
       <c r="Q66" s="6"/>
-      <c r="R66" s="300"/>
+      <c r="R66" s="289"/>
       <c r="S66" s="129"/>
       <c r="T66" s="130"/>
       <c r="U66" s="130"/>
@@ -17431,7 +17418,7 @@
       <c r="O67" s="256"/>
       <c r="P67" s="257"/>
       <c r="Q67" s="6"/>
-      <c r="R67" s="301"/>
+      <c r="R67" s="290"/>
       <c r="S67" s="129"/>
       <c r="T67" s="130"/>
       <c r="U67" s="130"/>
@@ -17472,7 +17459,7 @@
       <c r="O68" s="256"/>
       <c r="P68" s="257"/>
       <c r="Q68" s="6"/>
-      <c r="R68" s="302"/>
+      <c r="R68" s="291"/>
       <c r="S68" s="154"/>
       <c r="T68" s="6"/>
       <c r="U68" s="6"/>
@@ -17513,7 +17500,7 @@
       <c r="O69" s="256"/>
       <c r="P69" s="257"/>
       <c r="Q69" s="6"/>
-      <c r="R69" s="302"/>
+      <c r="R69" s="291"/>
       <c r="S69" s="154"/>
       <c r="T69" s="6"/>
       <c r="U69" s="6"/>

</xml_diff>